<commit_message>
Agrupamiento por avanzados y expertos.
</commit_message>
<xml_diff>
--- a/memberlist_attending.xlsx
+++ b/memberlist_attending.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="72" firstSheet="0" activeTab="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="72" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="200">
   <si>
     <t>Name</t>
   </si>
@@ -149,10 +149,7 @@
     <t>user 144486702</t>
   </si>
   <si>
-    <t>Stanford</t>
-  </si>
-  <si>
-    <t>CA</t>
+    <t>Stanford, CA</t>
   </si>
   <si>
     <t>01/05/2015</t>
@@ -260,10 +257,7 @@
     <t>user 154080962</t>
   </si>
   <si>
-    <t>New York</t>
-  </si>
-  <si>
-    <t>NY</t>
+    <t>New York, NY</t>
   </si>
   <si>
     <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/154080962/</t>
@@ -353,10 +347,7 @@
     <t>user 184772720</t>
   </si>
   <si>
-    <t>Pompano Beach</t>
-  </si>
-  <si>
-    <t>FL</t>
+    <t>Pompano Beach, </t>
   </si>
   <si>
     <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/184772720/</t>
@@ -545,42 +536,45 @@
     <t>Pablopda</t>
   </si>
   <si>
+    <t>San Francisco, CA</t>
+  </si>
+  <si>
+    <t>02/28/2015</t>
+  </si>
+  <si>
+    <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/30384032/</t>
+  </si>
+  <si>
+    <t>Patricio Del Boca</t>
+  </si>
+  <si>
+    <t>user 157866752</t>
+  </si>
+  <si>
+    <t>02/27/2015</t>
+  </si>
+  <si>
+    <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/157866752/</t>
+  </si>
+  <si>
+    <t>Pedro Pérez</t>
+  </si>
+  <si>
+    <t>user 183349310</t>
+  </si>
+  <si>
+    <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/183349310/</t>
+  </si>
+  <si>
+    <t>Roberto Allende</t>
+  </si>
+  <si>
+    <t>user 21813881</t>
+  </si>
+  <si>
     <t>San Francisco</t>
   </si>
   <si>
-    <t>02/28/2015</t>
-  </si>
-  <si>
-    <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/30384032/</t>
-  </si>
-  <si>
-    <t>Patricio Del Boca</t>
-  </si>
-  <si>
-    <t>user 157866752</t>
-  </si>
-  <si>
-    <t>02/27/2015</t>
-  </si>
-  <si>
-    <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/157866752/</t>
-  </si>
-  <si>
-    <t>Pedro Pérez</t>
-  </si>
-  <si>
-    <t>user 183349310</t>
-  </si>
-  <si>
-    <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/183349310/</t>
-  </si>
-  <si>
-    <t>Roberto Allende</t>
-  </si>
-  <si>
-    <t>user 21813881</t>
-  </si>
-  <si>
     <t>01/23/2015</t>
   </si>
   <si>
@@ -600,9 +594,6 @@
   </si>
   <si>
     <t>Juan Cruz</t>
-  </si>
-  <si>
-    <t>user 184770865</t>
   </si>
   <si>
     <t>http://www.meetup.com/Encuentros-Data-Science-Cordoba/members/184770865/</t>
@@ -631,30 +622,30 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="@" numFmtId="165"/>
   </numFmts>
   <fonts count="4">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -666,7 +657,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border diagonalDown="false" diagonalUp="false">
       <left/>
       <right/>
       <top/>
@@ -675,47 +666,41 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
+    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
+    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
+    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
+    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -727,33 +712,32 @@
   </sheetPr>
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I47" activeCellId="0" pane="topLeft" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.3520408163265"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.4591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.8520408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2959183673469"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.48469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.18367346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.29081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="67.2908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4745098039216"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="14.4274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5098039215686"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9764705882353"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.7450980392157"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.9098039215686"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5607843137255"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.3490196078431"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.0980392156863"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.53333333333333"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.2078431372549"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="6.32156862745098"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.6352941176471"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.7882352941176"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="0" width="67.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="11.5764705882353"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="1">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -812,7 +796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>19</v>
       </c>
@@ -865,7 +849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
         <v>26</v>
       </c>
@@ -918,7 +902,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="4">
       <c r="A4" s="0" t="s">
         <v>32</v>
       </c>
@@ -971,7 +955,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>37</v>
       </c>
@@ -1024,7 +1008,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>42</v>
       </c>
@@ -1037,55 +1021,52 @@
       <c r="E6" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="7">
+      <c r="A7" s="0" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>50</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>88304422</v>
@@ -1094,51 +1075,51 @@
         <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="8">
+      <c r="A8" s="0" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="B8" s="0" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>184772493</v>
@@ -1147,7 +1128,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>40</v>
@@ -1183,15 +1164,15 @@
         <v>24</v>
       </c>
       <c r="S8" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>184031174</v>
@@ -1200,7 +1181,7 @@
         <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>23</v>
@@ -1236,15 +1217,15 @@
         <v>24</v>
       </c>
       <c r="S9" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>18797921</v>
@@ -1256,48 +1237,48 @@
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S10" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B11" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>90710302</v>
@@ -1306,7 +1287,7 @@
         <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>40</v>
@@ -1342,15 +1323,15 @@
         <v>24</v>
       </c>
       <c r="S11" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>69</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>70</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>123599392</v>
@@ -1395,15 +1376,15 @@
         <v>24</v>
       </c>
       <c r="S12" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B13" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>95707422</v>
@@ -1448,15 +1429,15 @@
         <v>24</v>
       </c>
       <c r="S13" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>75</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>76</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>134793802</v>
@@ -1465,7 +1446,7 @@
         <v>21</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>23</v>
@@ -1501,71 +1482,68 @@
         <v>24</v>
       </c>
       <c r="S14" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="B15" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>154080962</v>
       </c>
       <c r="E15" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="16">
+      <c r="A16" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R15" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="S15" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="T15" s="0" t="s">
+      <c r="B16" s="0" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>183396449</v>
@@ -1577,48 +1555,48 @@
         <v>34</v>
       </c>
       <c r="G16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="17">
+      <c r="A17" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R16" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16" s="0" t="s">
+      <c r="B17" s="0" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>156890362</v>
@@ -1627,7 +1605,7 @@
         <v>21</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>40</v>
@@ -1663,15 +1641,15 @@
         <v>24</v>
       </c>
       <c r="S17" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="18">
+      <c r="A18" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>93</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>184516750</v>
@@ -1680,7 +1658,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>23</v>
@@ -1716,15 +1694,15 @@
         <v>24</v>
       </c>
       <c r="S18" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="19">
+      <c r="A19" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>183577530</v>
@@ -1769,15 +1747,15 @@
         <v>24</v>
       </c>
       <c r="S19" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="20">
+      <c r="A20" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>100</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>184772995</v>
@@ -1786,10 +1764,10 @@
         <v>21</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>1</v>
@@ -1822,68 +1800,68 @@
         <v>24</v>
       </c>
       <c r="S20" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="21">
+      <c r="A21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>103</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>184080440</v>
       </c>
       <c r="E21" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R21" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S21" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="F21" s="1" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="22">
+      <c r="A22" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q21" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S21" s="0" t="s">
+      <c r="B22" s="0" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>108</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>183334845</v>
@@ -1892,10 +1870,10 @@
         <v>21</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>1</v>
@@ -1928,71 +1906,68 @@
         <v>24</v>
       </c>
       <c r="S22" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="23">
+      <c r="A23" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>111</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>184772720</v>
       </c>
       <c r="E23" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="T23" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="24">
+      <c r="A24" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R23" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="S23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="T23" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>115</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>116</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>183941822</v>
@@ -2001,51 +1976,51 @@
         <v>21</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="25">
+      <c r="A25" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P24" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q24" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R24" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S24" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>120</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>184052161</v>
@@ -2054,51 +2029,51 @@
         <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="26">
+      <c r="A26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>121</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P25" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q25" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R25" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S25" s="0" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>124</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>183601192</v>
@@ -2107,10 +2082,10 @@
         <v>21</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>1</v>
@@ -2143,15 +2118,15 @@
         <v>24</v>
       </c>
       <c r="S26" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>122</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>183815772</v>
@@ -2160,7 +2135,7 @@
         <v>21</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>23</v>
@@ -2196,15 +2171,15 @@
         <v>24</v>
       </c>
       <c r="S27" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>80192692</v>
@@ -2213,7 +2188,7 @@
         <v>21</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>40</v>
@@ -2249,15 +2224,15 @@
         <v>24</v>
       </c>
       <c r="S28" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>129</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>183456245</v>
@@ -2266,10 +2241,10 @@
         <v>21</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>1</v>
@@ -2302,15 +2277,15 @@
         <v>24</v>
       </c>
       <c r="S29" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>132</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>177738162</v>
@@ -2319,51 +2294,51 @@
         <v>21</v>
       </c>
       <c r="F30" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R30" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="31">
+      <c r="A31" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P30" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q30" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R30" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S30" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>140</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>141</v>
       </c>
       <c r="D31" s="0" t="n">
         <v>183316808</v>
@@ -2375,48 +2350,48 @@
         <v>22</v>
       </c>
       <c r="G31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q31" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R31" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S31" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="32">
+      <c r="A32" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>142</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q31" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S31" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>145</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>183394684</v>
@@ -2461,15 +2436,15 @@
         <v>24</v>
       </c>
       <c r="S32" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>143</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>184546859</v>
@@ -2478,60 +2453,60 @@
         <v>21</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q33" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R33" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="34">
+      <c r="A34" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>149</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="I33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J33" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P33" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q33" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R33" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S33" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>151</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>152</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>14446359</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>40</v>
@@ -2567,21 +2542,21 @@
         <v>24</v>
       </c>
       <c r="S34" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>151</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>22485641</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>34</v>
@@ -2620,15 +2595,15 @@
         <v>24</v>
       </c>
       <c r="S35" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>154</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>184776796</v>
@@ -2637,10 +2612,10 @@
         <v>21</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I36" s="0" t="n">
         <v>1</v>
@@ -2673,15 +2648,15 @@
         <v>24</v>
       </c>
       <c r="S36" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>157</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>110634352</v>
@@ -2690,63 +2665,63 @@
         <v>21</v>
       </c>
       <c r="F37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q37" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S37" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="38">
+      <c r="A38" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>163</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P37" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q37" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R37" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S37" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>166</v>
       </c>
       <c r="D38" s="0" t="n">
         <v>104888702</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I38" s="0" t="n">
         <v>5</v>
@@ -2779,15 +2754,15 @@
         <v>24</v>
       </c>
       <c r="S38" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>167</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>184775141</v>
@@ -2796,7 +2771,7 @@
         <v>21</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>40</v>
@@ -2832,30 +2807,27 @@
         <v>24</v>
       </c>
       <c r="S39" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>170</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>30384032</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F40" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>45</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>5</v>
@@ -2888,68 +2860,68 @@
         <v>24</v>
       </c>
       <c r="T40" s="0" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>175</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>157866752</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="P41" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="R41" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="42">
+      <c r="A42" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>181</v>
-      </c>
-      <c r="I41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J41" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P41" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q41" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R41" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="S41" s="0" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>184</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>183349310</v>
@@ -2958,10 +2930,10 @@
         <v>21</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I42" s="0" t="n">
         <v>1</v>
@@ -2994,71 +2966,68 @@
         <v>24</v>
       </c>
       <c r="S42" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>182</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>21813881</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>176</v>
-      </c>
-      <c r="F43" s="0" t="s">
-        <v>45</v>
+        <v>185</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H43" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q43" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R43" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S43" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="T43" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="44">
+      <c r="A44" s="0" t="s">
         <v>188</v>
       </c>
-      <c r="J43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K43" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q43" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R43" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="S43" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="T43" s="0" t="s">
+      <c r="B44" s="0" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>191</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>161536292</v>
@@ -3067,7 +3036,7 @@
         <v>21</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>29</v>
@@ -3103,83 +3072,80 @@
         <v>24</v>
       </c>
       <c r="S44" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="45">
+      <c r="A45" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="D45" s="0" t="n">
+        <v>184770865</v>
+      </c>
+      <c r="E45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q45" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="R45" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="S45" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="T45" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="B45" s="0" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="46">
+      <c r="A46" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="B46" s="0" t="s">
         <v>195</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>184770865</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="N45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="O45" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="P45" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q45" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="R45" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="S45" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="T45" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>198</v>
       </c>
       <c r="D46" s="0" t="n">
         <v>10300630</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I46" s="0" t="n">
         <v>1</v>
@@ -3212,15 +3178,15 @@
         <v>24</v>
       </c>
       <c r="S46" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>196</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.6" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>73867602</v>
@@ -3229,10 +3195,10 @@
         <v>21</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I47" s="0" t="n">
         <v>1</v>
@@ -3265,13 +3231,13 @@
         <v>24</v>
       </c>
       <c r="S47" s="0" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>